<commit_message>
Committed on 07/12/2018:19:10:00PM By Karthikeyan Rajendran
</commit_message>
<xml_diff>
--- a/data/Input_Data_Targeted_Email_Marketing_Campaigns.xlsx
+++ b/data/Input_Data_Targeted_Email_Marketing_Campaigns.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="8370" windowWidth="20385"/>
+    <workbookView windowWidth="20385" windowHeight="8370" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Web_Page_Test_Mobile" r:id="rId1" sheetId="1"/>
-    <sheet name="Web_Page_Test_Desktop" r:id="rId2" sheetId="2"/>
-    <sheet name="Page_Insight" r:id="rId3" sheetId="3"/>
-    <sheet name="GT_metrix" r:id="rId4" sheetId="5"/>
-    <sheet name="Page_Count" r:id="rId5" sheetId="4"/>
+    <sheet name="Web_Page_Test_Mobile" sheetId="1" r:id="rId1"/>
+    <sheet name="Web_Page_Test_Desktop" sheetId="2" r:id="rId2"/>
+    <sheet name="Page_Insight" sheetId="3" r:id="rId3"/>
+    <sheet name="GT_metrix" sheetId="5" r:id="rId4"/>
+    <sheet name="Page_Count" sheetId="4" r:id="rId5"/>
+    <sheet name="Mobile_Friendliness" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:C11"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63">
   <si>
     <t>Urls</t>
   </si>
@@ -202,6 +203,12 @@
   </si>
   <si>
     <t>5,100</t>
+  </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
+  <si>
+    <t>Explaination</t>
   </si>
 </sst>
 </file>
@@ -209,10 +216,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -237,15 +244,33 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -268,31 +293,45 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -306,73 +345,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -380,6 +352,41 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -402,187 +409,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -592,6 +599,19 @@
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -612,15 +632,32 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -629,6 +666,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,16 +690,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -677,278 +723,242 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="179">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="178">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="10" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="24" fontId="0" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="20" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="21" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="17" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="14" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="34" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="14" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="9" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="2" numFmtId="9" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
-    <cellStyle builtinId="3" name="Comma" xfId="2"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="4" name="Currency" xfId="5"/>
-    <cellStyle builtinId="5" name="Percent" xfId="6"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="7"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="8"/>
-    <cellStyle builtinId="10" name="Note" xfId="9"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="10"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="11"/>
-    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="12"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
-    <cellStyle builtinId="15" name="Title" xfId="16"/>
-    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
-    <cellStyle builtinId="20" name="Input" xfId="21"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
-    <cellStyle builtinId="26" name="Good" xfId="23"/>
-    <cellStyle builtinId="21" name="Output" xfId="24"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
-    <cellStyle builtinId="25" name="Total" xfId="28"/>
-    <cellStyle builtinId="27" name="Bad" xfId="29"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
-    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -962,10 +972,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1129,21 +1139,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1160,7 +1170,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1213,29 +1223,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.2857142857143" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="21.2857142857143" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="80.8571428571429" collapsed="false"/>
+    <col min="1" max="1" width="34.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="21.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="80.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="30" spans="1:3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1310,15 +1320,15 @@
       <c r="C11" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:E11"/>
@@ -1326,27 +1336,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="9.85714285714286" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="8.85714285714286" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="14.0" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="89.2857142857143" collapsed="false"/>
+    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="9.85714285714286" customWidth="1"/>
+    <col min="3" max="3" width="8.85714285714286" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="89.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="30" spans="1:5">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1441,34 +1451,34 @@
       <c r="E11" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="12.2857142857143" collapsed="false"/>
+    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="12.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1486,8 +1496,8 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
       <c r="D3" t="s">
         <v>19</v>
       </c>
@@ -1496,22 +1506,22 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="6"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
@@ -1528,15 +1538,15 @@
       <c r="C8" s="3"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1544,23 +1554,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.2857142857143" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.1428571428571" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="65.0" collapsed="false"/>
+    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="12.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="11.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="21" r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="21" customHeight="1" spans="1:4">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1705,15 +1715,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
@@ -1721,15 +1731,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="13.2857142857143" collapsed="false"/>
+    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="13.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1814,7 +1824,89 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="10.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes in config by Manika prabu on 14.12.2018.13.37
</commit_message>
<xml_diff>
--- a/data/Input_Data_Targeted_Email_Marketing_Campaigns.xlsx
+++ b/data/Input_Data_Targeted_Email_Marketing_Campaigns.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370" activeTab="5"/>
+    <workbookView windowHeight="8340" windowWidth="20295"/>
   </bookViews>
   <sheets>
-    <sheet name="Web_Page_Test_Mobile" sheetId="1" r:id="rId1"/>
-    <sheet name="Web_Page_Test_Desktop" sheetId="2" r:id="rId2"/>
-    <sheet name="Page_Insight" sheetId="3" r:id="rId3"/>
-    <sheet name="GT_metrix" sheetId="5" r:id="rId4"/>
-    <sheet name="Page_Count" sheetId="4" r:id="rId5"/>
-    <sheet name="Mobile_Friendliness" sheetId="6" r:id="rId6"/>
+    <sheet name="Web_Page_Test_Mobile" r:id="rId1" sheetId="1"/>
+    <sheet name="Web_Page_Test_Desktop" r:id="rId2" sheetId="2"/>
+    <sheet name="Page_Insight" r:id="rId3" sheetId="3"/>
+    <sheet name="GT_metrix" r:id="rId4" sheetId="5"/>
+    <sheet name="Page_Count" r:id="rId5" sheetId="4"/>
+    <sheet name="Mobile_Friendliness" r:id="rId6" sheetId="6"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:C11"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
   <si>
     <t>Urls</t>
   </si>
@@ -91,13 +91,70 @@
     <t>URL</t>
   </si>
   <si>
+    <t>No. Of Pages</t>
+  </si>
+  <si>
+    <t>21,900</t>
+  </si>
+  <si>
+    <t>356</t>
+  </si>
+  <si>
+    <t>22,400</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>2,400</t>
+  </si>
+  <si>
+    <t>831</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>930</t>
+  </si>
+  <si>
+    <t>5,110</t>
+  </si>
+  <si>
+    <t>4,910</t>
+  </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
+  <si>
+    <t>Explaination</t>
+  </si>
+  <si>
+    <t>This page is mobile friendly</t>
+  </si>
+  <si>
+    <t>Viewport configured correctly,Page content fits device width,Text on the page is readable,Links and tap targets are sufficiently large and touch-friendly</t>
+  </si>
+  <si>
+    <t>Viewport configured correctly,Page content fits device width,Text on the page is readable,Links and tap targets are sufficiently large and touch-friendly,Some resources on the page are blocked by robots.txt configuration</t>
+  </si>
+  <si>
+    <t>41%</t>
+  </si>
+  <si>
+    <t>97%</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.sfwmd.gov/IzknQnjH</t>
+  </si>
+  <si>
     <t>F(32%)</t>
   </si>
   <si>
     <t>D(65%)</t>
   </si>
   <si>
-    <t>https://gtmetrix.com/reports/www.sfwmd.gov/QXNTpbHt</t>
+    <t>https://gtmetrix.com/reports/www.nicb.org/rCl1xxSz</t>
   </si>
   <si>
     <t>A(92%)</t>
@@ -106,109 +163,82 @@
     <t>B(83%)</t>
   </si>
   <si>
-    <t>https://gtmetrix.com/reports/www.nicb.org/ODOZ4yyE</t>
+    <t>https://gtmetrix.com/reports/www.boston.gov/InY47CX5</t>
   </si>
   <si>
     <t>F(27%)</t>
   </si>
   <si>
-    <t>B(84%)</t>
-  </si>
-  <si>
-    <t>https://gtmetrix.com/reports/www.boston.gov/Je4BaCPb</t>
+    <t>B(82%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.allsouth.org/kpJQPugC</t>
   </si>
   <si>
     <t>F(13%)</t>
   </si>
   <si>
-    <t>https://gtmetrix.com/reports/www.allsouth.org/pofOIELM</t>
+    <t>https://gtmetrix.com/reports/www.rutheckerdhall.com/4wrOGB75</t>
   </si>
   <si>
     <t>F(35%)</t>
   </si>
   <si>
+    <t>E(50%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.shelbyvote.com/cmJZQJQR</t>
+  </si>
+  <si>
+    <t>E(55%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/gefen.com/DPEvHV4k</t>
+  </si>
+  <si>
     <t>F(49%)</t>
   </si>
   <si>
-    <t>https://gtmetrix.com/reports/www.rutheckerdhall.com/NV2NIPni</t>
-  </si>
-  <si>
-    <t>E(50%)</t>
-  </si>
-  <si>
-    <t>E(55%)</t>
-  </si>
-  <si>
-    <t>https://gtmetrix.com/reports/www.shelbyvote.com/bXGZAROT</t>
-  </si>
-  <si>
-    <t>B(87%)</t>
-  </si>
-  <si>
-    <t>D(64%)</t>
-  </si>
-  <si>
-    <t>https://gtmetrix.com/reports/how.drsusanloveresearch.org/w6DILNfU</t>
-  </si>
-  <si>
     <t>C(74%)</t>
   </si>
   <si>
-    <t>https://gtmetrix.com/reports/gefen.com/g6cCx9jJ</t>
+    <t>https://gtmetrix.com/reports/www.valleymetro.org/vaILbFNa</t>
+  </si>
+  <si>
+    <t>D(60%)</t>
+  </si>
+  <si>
+    <t>D(63%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.lbcc.edu/77l1VdR9</t>
   </si>
   <si>
     <t>E(59%)</t>
   </si>
   <si>
-    <t>D(63%)</t>
-  </si>
-  <si>
-    <t>https://gtmetrix.com/reports/www.valleymetro.org/kJ6fyeBN</t>
-  </si>
-  <si>
-    <t>E(58%)</t>
-  </si>
-  <si>
-    <t>https://gtmetrix.com/reports/www.lbcc.edu/X6bh6g65</t>
-  </si>
-  <si>
-    <t>No. Of Pages</t>
-  </si>
-  <si>
-    <t>22,100</t>
-  </si>
-  <si>
-    <t>285</t>
-  </si>
-  <si>
-    <t>19,500</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>2,380</t>
-  </si>
-  <si>
-    <t>1,150</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>891</t>
-  </si>
-  <si>
-    <t>5,220</t>
-  </si>
-  <si>
-    <t>5,100</t>
-  </si>
-  <si>
-    <t>Conclusion</t>
-  </si>
-  <si>
-    <t>Explaination</t>
+    <t>https://www.webpagetest.org/result/181207_VY_998ade7fda1001d515abd6cb0b80ab85/</t>
+  </si>
+  <si>
+    <t>3.48</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181207_9C_e70ca0d569061eb9093871f73ae492ae/</t>
+  </si>
+  <si>
+    <t>4.99</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181207_9F_77e325c6960bb21bfae1402e9507299b/</t>
+  </si>
+  <si>
+    <t>12.44</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181207_4J_4962448db2261c02a1ef4b6990aad023/</t>
+  </si>
+  <si>
+    <t>8.56</t>
   </si>
 </sst>
 </file>
@@ -218,8 +248,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -244,6 +274,34 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -262,9 +320,25 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -276,6 +350,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -292,9 +373,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -309,84 +405,18 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -409,13 +439,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,25 +601,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,139 +619,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -631,21 +661,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -672,35 +687,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -723,6 +714,45 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -730,235 +760,235 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="179">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="178">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="8" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="19" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="14" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="30" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="30" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="0" fontId="21" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="34" fontId="20" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="2" numFmtId="9" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="2" numFmtId="9" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="3" fontId="2" numFmtId="9" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="6"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="7"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="8"/>
+    <cellStyle builtinId="10" name="Note" xfId="9"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="10"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="11"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="12"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
+    <cellStyle builtinId="20" name="Input" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="26" name="Good" xfId="23"/>
+    <cellStyle builtinId="21" name="Output" xfId="24"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
+    <cellStyle builtinId="25" name="Total" xfId="28"/>
+    <cellStyle builtinId="27" name="Bad" xfId="29"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -972,10 +1002,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1139,21 +1169,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1170,7 +1200,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1223,22 +1253,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="34.2857142857143" customWidth="1"/>
-    <col min="2" max="2" width="21.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="80.8571428571429" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="34.2857142857143" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="21.2857142857143" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="80.8571428571429" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" spans="1:3">
+    <row ht="30" r="1" spans="1:3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1253,8 +1283,12 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
@@ -1274,22 +1308,34 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
@@ -1320,15 +1366,15 @@
       <c r="C11" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:E11"/>
@@ -1336,14 +1382,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="9.85714285714286" customWidth="1"/>
-    <col min="3" max="3" width="8.85714285714286" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="89.2857142857143" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="9.85714285714286" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="8.85714285714286" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="89.2857142857143" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" spans="1:5">
+    <row ht="30" r="1" spans="1:5">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1451,24 +1497,24 @@
       <c r="E11" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B2" sqref="B2:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3" outlineLevelRow="7"/>
   <cols>
-    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="12.2857142857143" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="12.2857142857143" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1486,8 +1532,12 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D2" t="s">
         <v>19</v>
       </c>
@@ -1538,29 +1588,29 @@
       <c r="C8" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B2" sqref="B2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="12.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="11.1428571428571" customWidth="1"/>
-    <col min="4" max="4" width="65" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="12.2857142857143" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="11.1428571428571" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="65.0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1" spans="1:4">
+    <row customHeight="1" ht="21" r="1" spans="1:4">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1579,13 +1629,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1593,13 +1643,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1607,13 +1657,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1621,13 +1671,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1635,13 +1685,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1649,41 +1699,35 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1691,13 +1735,13 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1705,34 +1749,34 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="13.2857142857143" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="13.2857142857143" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1740,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1748,7 +1792,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1756,7 +1800,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1764,7 +1808,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1772,7 +1816,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1780,7 +1824,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1788,7 +1832,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1796,7 +1840,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1804,7 +1848,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1812,7 +1856,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1820,29 +1864,29 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2" outlineLevelRow="7"/>
   <cols>
-    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="10.4285714285714" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="10.4285714285714" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1850,25 +1894,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row ht="38.25" r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
@@ -1884,29 +1936,41 @@
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:3">
+    <row ht="38.25" r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
+      <c r="B8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>